<commit_message>
revised quiz data convert
</commit_message>
<xml_diff>
--- a/app/assets/javascripts/quiz_data/quiz1.xlsx
+++ b/app/assets/javascripts/quiz_data/quiz1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t>What is the maximum number of words per article?</t>
   </si>
@@ -238,7 +238,13 @@
     <t>Styles</t>
   </si>
   <si>
-    <t>Test your --skilz-- skills</t>
+    <t>secretsauce.com/:track/:page/</t>
+  </si>
+  <si>
+    <t>styles</t>
+  </si>
+  <si>
+    <t>Test your --$kilz-- skills</t>
   </si>
 </sst>
 </file>
@@ -316,7 +322,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -340,8 +346,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -352,16 +362,24 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -373,6 +391,8 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -384,6 +404,8 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -716,7 +738,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -730,66 +752,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" ht="23">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="23">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="23">
+      <c r="A4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" ht="23">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="B4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="23">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="8" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>